<commit_message>
ATUALIZAÇÃO TABELA DE CLIENTES
</commit_message>
<xml_diff>
--- a/data/clientes.xlsx
+++ b/data/clientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael\tickets_entrega\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16403CC-3396-43B9-803B-FE2C1838B987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94EE6B56-FB49-4BE6-A236-4408DA99CE64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{52E17E58-EB7C-41A6-A909-4B7E1F6FB134}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="98">
   <si>
     <t>Cliente</t>
   </si>
@@ -311,6 +311,9 @@
   </si>
   <si>
     <t>eurafaelmedeiros@gmail.com</t>
+  </si>
+  <si>
+    <t>FAST HORIZON LOGISTICA INTELIGENTE LTDA</t>
   </si>
 </sst>
 </file>
@@ -891,10 +894,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D1A6003-AD6B-420F-B8FD-891612A2B579}" name="Tabela2" displayName="Tabela2" ref="A1:D45" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D45" xr:uid="{0D1A6003-AD6B-420F-B8FD-891612A2B579}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D44">
-    <sortCondition ref="A1:A44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D1A6003-AD6B-420F-B8FD-891612A2B579}" name="Tabela2" displayName="Tabela2" ref="A1:D46" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D46" xr:uid="{0D1A6003-AD6B-420F-B8FD-891612A2B579}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D45">
+    <sortCondition ref="A1:A45"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{8DC57E86-0FB3-40B3-BDF2-C3CA9F749020}" name="Cliente" dataDxfId="3"/>
@@ -1223,10 +1226,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F76EBC0C-1615-4DFC-BD6E-22E70D5FB3B8}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1489,49 +1492,45 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>57</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>61</v>
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>14</v>
@@ -1545,7 +1544,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>14</v>
@@ -1559,93 +1558,99 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>75</v>
+      <c r="C27" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" t="s">
-        <v>9</v>
+        <v>33</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B29" t="s">
         <v>9</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>82</v>
+      <c r="C30" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>39</v>
+        <v>9</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>39</v>
@@ -1653,55 +1658,49 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>61</v>
+        <v>83</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>63</v>
@@ -1709,13 +1708,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>63</v>
@@ -1723,13 +1722,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>63</v>
@@ -1737,136 +1736,150 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B40" t="s">
-        <v>9</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>90</v>
+        <v>46</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B41" t="s">
         <v>9</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="B42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>59</v>
+      <c r="C44" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>95</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C11" r:id="rId1" xr:uid="{D9003C5C-3976-4A85-84F9-9B237DD2F850}"/>
-    <hyperlink ref="C38" r:id="rId2" xr:uid="{D48B5608-77E8-4655-B5DC-33A18BD1112D}"/>
-    <hyperlink ref="C37" r:id="rId3" xr:uid="{F7DADD4D-52AC-45C3-B72C-6BA80BEFDBF5}"/>
-    <hyperlink ref="C36" r:id="rId4" xr:uid="{976065DB-E912-4BC6-90E8-7DE9A870855B}"/>
-    <hyperlink ref="C35" r:id="rId5" xr:uid="{FAF31D9C-BAAD-4026-AF42-A374AAB19B27}"/>
-    <hyperlink ref="C24" r:id="rId6" xr:uid="{0F0E793E-D3E0-4501-92AA-0FBE0ACA9582}"/>
-    <hyperlink ref="C23" r:id="rId7" xr:uid="{C4A916CE-E516-463B-9CC9-9E1417330B2C}"/>
-    <hyperlink ref="C22" r:id="rId8" xr:uid="{2FF926B0-9E5B-43BE-8215-37A1B7538235}"/>
+    <hyperlink ref="C39" r:id="rId2" xr:uid="{D48B5608-77E8-4655-B5DC-33A18BD1112D}"/>
+    <hyperlink ref="C38" r:id="rId3" xr:uid="{F7DADD4D-52AC-45C3-B72C-6BA80BEFDBF5}"/>
+    <hyperlink ref="C37" r:id="rId4" xr:uid="{976065DB-E912-4BC6-90E8-7DE9A870855B}"/>
+    <hyperlink ref="C36" r:id="rId5" xr:uid="{FAF31D9C-BAAD-4026-AF42-A374AAB19B27}"/>
+    <hyperlink ref="C25" r:id="rId6" xr:uid="{0F0E793E-D3E0-4501-92AA-0FBE0ACA9582}"/>
+    <hyperlink ref="C24" r:id="rId7" xr:uid="{C4A916CE-E516-463B-9CC9-9E1417330B2C}"/>
+    <hyperlink ref="C23" r:id="rId8" xr:uid="{2FF926B0-9E5B-43BE-8215-37A1B7538235}"/>
     <hyperlink ref="C18" r:id="rId9" xr:uid="{D4E79195-E761-4206-AE05-FB85E48B886F}"/>
     <hyperlink ref="C10" r:id="rId10" xr:uid="{50DB6CC9-A8ED-488E-95E8-A8C016D2DEEF}"/>
     <hyperlink ref="C9" r:id="rId11" xr:uid="{8C70D519-E5C6-4DB6-B04E-24A429A455E6}"/>
     <hyperlink ref="C8" r:id="rId12" xr:uid="{EEE992FD-9460-458C-9A17-BA90502683BC}"/>
-    <hyperlink ref="C21" r:id="rId13" xr:uid="{056E78F0-5BA0-45A9-A268-ADCAFA6EA41F}"/>
-    <hyperlink ref="C34" r:id="rId14" xr:uid="{22C516E5-3522-45BE-828E-C5F67E908608}"/>
+    <hyperlink ref="C22" r:id="rId13" xr:uid="{056E78F0-5BA0-45A9-A268-ADCAFA6EA41F}"/>
+    <hyperlink ref="C35" r:id="rId14" xr:uid="{22C516E5-3522-45BE-828E-C5F67E908608}"/>
     <hyperlink ref="C6" r:id="rId15" xr:uid="{443B64A5-35EF-49EF-969A-F6923542F77D}"/>
     <hyperlink ref="C12" r:id="rId16" xr:uid="{1164D05E-041D-4217-8522-AF445ADB09A8}"/>
-    <hyperlink ref="C20" r:id="rId17" xr:uid="{890ACA54-A4DD-472D-A6EE-EA4482B06391}"/>
-    <hyperlink ref="C28" r:id="rId18" xr:uid="{D7101A34-D1A3-4576-9715-A05F201ED4A8}"/>
-    <hyperlink ref="D28" r:id="rId19" xr:uid="{23320200-0AE3-4806-AE7D-DDE9471D6290}"/>
-    <hyperlink ref="C29" r:id="rId20" xr:uid="{29F7C5FB-B2C6-4E00-90CE-525A2A52EDE7}"/>
-    <hyperlink ref="D29" r:id="rId21" xr:uid="{A255BF9E-0F74-4763-8072-A35F58A421D3}"/>
-    <hyperlink ref="C40" r:id="rId22" xr:uid="{C1500DF4-96DA-4ED7-B5AB-D464962FC05C}"/>
-    <hyperlink ref="D40" r:id="rId23" xr:uid="{B6B748D9-B355-4616-9896-661673A87DBD}"/>
-    <hyperlink ref="C41" r:id="rId24" xr:uid="{7A695E45-2E79-41FD-B3AE-3A78288E0DC0}"/>
-    <hyperlink ref="D41" r:id="rId25" xr:uid="{FD7326B4-77F0-4BF6-BF28-562E394B257B}"/>
-    <hyperlink ref="C30" r:id="rId26" xr:uid="{D66CB11B-C3E4-4678-B457-E4BCE976FC62}"/>
-    <hyperlink ref="D30" r:id="rId27" xr:uid="{734E64F0-D062-4D4A-A517-287ADF2A867B}"/>
-    <hyperlink ref="C33" r:id="rId28" xr:uid="{F579E60C-F1F2-4554-B547-9286B7F2B3EF}"/>
+    <hyperlink ref="C21" r:id="rId17" xr:uid="{890ACA54-A4DD-472D-A6EE-EA4482B06391}"/>
+    <hyperlink ref="C29" r:id="rId18" xr:uid="{D7101A34-D1A3-4576-9715-A05F201ED4A8}"/>
+    <hyperlink ref="D29" r:id="rId19" xr:uid="{23320200-0AE3-4806-AE7D-DDE9471D6290}"/>
+    <hyperlink ref="C30" r:id="rId20" xr:uid="{29F7C5FB-B2C6-4E00-90CE-525A2A52EDE7}"/>
+    <hyperlink ref="D30" r:id="rId21" xr:uid="{A255BF9E-0F74-4763-8072-A35F58A421D3}"/>
+    <hyperlink ref="C41" r:id="rId22" xr:uid="{C1500DF4-96DA-4ED7-B5AB-D464962FC05C}"/>
+    <hyperlink ref="D41" r:id="rId23" xr:uid="{B6B748D9-B355-4616-9896-661673A87DBD}"/>
+    <hyperlink ref="C42" r:id="rId24" xr:uid="{7A695E45-2E79-41FD-B3AE-3A78288E0DC0}"/>
+    <hyperlink ref="D42" r:id="rId25" xr:uid="{FD7326B4-77F0-4BF6-BF28-562E394B257B}"/>
+    <hyperlink ref="C31" r:id="rId26" xr:uid="{D66CB11B-C3E4-4678-B457-E4BCE976FC62}"/>
+    <hyperlink ref="D31" r:id="rId27" xr:uid="{734E64F0-D062-4D4A-A517-287ADF2A867B}"/>
+    <hyperlink ref="C34" r:id="rId28" xr:uid="{F579E60C-F1F2-4554-B547-9286B7F2B3EF}"/>
     <hyperlink ref="C7" r:id="rId29" xr:uid="{50748FF0-CD13-496A-B740-EFDCD7C21667}"/>
     <hyperlink ref="C13" r:id="rId30" xr:uid="{227F93B3-255B-46D6-AF4E-63A6FCA82B36}"/>
     <hyperlink ref="C14" r:id="rId31" xr:uid="{6B2D872C-DD3D-4966-A510-2E0C0BACE286}"/>
     <hyperlink ref="C19" r:id="rId32" xr:uid="{B7C0B1B5-7D60-46C7-BB4E-8F7A768593D0}"/>
-    <hyperlink ref="C26" r:id="rId33" xr:uid="{6805F0C2-147C-4CD1-A4FC-6775B1D94F1B}"/>
-    <hyperlink ref="C27" r:id="rId34" xr:uid="{C18472B2-6AF0-49D3-9429-576E9366C004}"/>
+    <hyperlink ref="C27" r:id="rId33" xr:uid="{6805F0C2-147C-4CD1-A4FC-6775B1D94F1B}"/>
+    <hyperlink ref="C28" r:id="rId34" xr:uid="{C18472B2-6AF0-49D3-9429-576E9366C004}"/>
     <hyperlink ref="D19" r:id="rId35" xr:uid="{FBF0CF62-8321-48C7-98A0-DF47918A71B3}"/>
-    <hyperlink ref="C43" r:id="rId36" xr:uid="{51B18494-45AA-4DB2-9536-B6FDE6D9ADB0}"/>
-    <hyperlink ref="C44" r:id="rId37" xr:uid="{048ADA5B-05B1-453F-9912-7B7D23218E3D}"/>
+    <hyperlink ref="C44" r:id="rId36" xr:uid="{51B18494-45AA-4DB2-9536-B6FDE6D9ADB0}"/>
+    <hyperlink ref="C45" r:id="rId37" xr:uid="{048ADA5B-05B1-453F-9912-7B7D23218E3D}"/>
     <hyperlink ref="D13" r:id="rId38" xr:uid="{8683A207-A70F-4C9F-AE2A-2B318546B7EF}"/>
     <hyperlink ref="D14" r:id="rId39" xr:uid="{84583E90-903B-4E5C-A55D-9372A24E34AA}"/>
-    <hyperlink ref="D43" r:id="rId40" xr:uid="{BBF1962D-68BB-4E98-B4A0-579D33DE5E53}"/>
+    <hyperlink ref="D44" r:id="rId40" xr:uid="{BBF1962D-68BB-4E98-B4A0-579D33DE5E53}"/>
     <hyperlink ref="D18" r:id="rId41" display="biri@biri.ind.br" xr:uid="{ACCA0632-2092-4676-91B4-E4D5E5D00113}"/>
     <hyperlink ref="D9:D12" r:id="rId42" display="biri@biri.ind.br" xr:uid="{A5222699-7918-44C3-A7B6-8C4DAE6DCD56}"/>
-    <hyperlink ref="D45" r:id="rId43" xr:uid="{DCBE0475-9B46-472A-8E91-D86C88ED948A}"/>
-    <hyperlink ref="C45" r:id="rId44" xr:uid="{81E2970F-6E36-46FF-9AA3-C72ABB168012}"/>
+    <hyperlink ref="D46" r:id="rId43" xr:uid="{DCBE0475-9B46-472A-8E91-D86C88ED948A}"/>
+    <hyperlink ref="C46" r:id="rId44" xr:uid="{81E2970F-6E36-46FF-9AA3-C72ABB168012}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">

</xml_diff>